<commit_message>
feat(#387): Updating master template spreadsheet
</commit_message>
<xml_diff>
--- a/app/public/master_template.xlsx
+++ b/app/public/master_template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="718">
   <si>
     <t>COLOR LEGENDS</t>
   </si>
@@ -1352,7 +1352,13 @@
     <t>Test Conditions - Temperature</t>
   </si>
   <si>
+    <t>only fill in when it's frequency dependence</t>
+  </si>
+  <si>
     <t>Test Conditions - Frequency</t>
+  </si>
+  <si>
+    <t>only fill in when it's temperature dependence</t>
   </si>
   <si>
     <t>Real permittivity</t>
@@ -1608,10 +1614,16 @@
     <t>Width</t>
   </si>
   <si>
+    <t>pixel</t>
+  </si>
+  <si>
     <t>Height</t>
   </si>
   <si>
     <t>Depth</t>
+  </si>
+  <si>
+    <t>bit</t>
   </si>
   <si>
     <t>Preprocessing</t>
@@ -1697,6 +1709,9 @@
     <t>Min frequency</t>
   </si>
   <si>
+    <t>Hz</t>
+  </si>
+  <si>
     <t>Max frequency</t>
   </si>
   <si>
@@ -1751,10 +1766,16 @@
     <t>Scale - nm per RVE length unit</t>
   </si>
   <si>
+    <t>nm/pi(vo)xel</t>
+  </si>
+  <si>
     <t>2D RVE</t>
   </si>
   <si>
     <t>3D RVE</t>
+  </si>
+  <si>
+    <t>voxel</t>
   </si>
   <si>
     <t>Length</t>
@@ -2825,7 +2846,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="52">
     <border/>
     <border>
       <left/>
@@ -3232,6 +3253,11 @@
       </bottom>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
       <left/>
       <top/>
       <bottom/>
@@ -3271,7 +3297,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="165">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -3626,6 +3652,9 @@
     <xf borderId="45" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="46" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="22" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -3650,6 +3679,9 @@
     <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="46" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf borderId="38" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -3659,13 +3691,13 @@
     <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="46" fillId="7" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="47" fillId="7" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="47" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="48" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="48" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="49" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="1" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3686,7 +3718,7 @@
     <xf borderId="44" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="49" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="50" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="19" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3713,13 +3745,13 @@
     <xf borderId="45" fillId="2" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="50" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="51" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="49" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="50" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="18" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -5083,12 +5115,12 @@
     </row>
     <row r="2" ht="60.75" customHeight="1">
       <c r="A2" s="113" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="30" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>54</v>
@@ -5114,7 +5146,7 @@
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -5125,7 +5157,7 @@
     </row>
     <row r="6">
       <c r="A6" s="16" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -5146,7 +5178,7 @@
     </row>
     <row r="8">
       <c r="A8" s="16" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -5157,7 +5189,7 @@
     </row>
     <row r="9">
       <c r="A9" s="16" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -5168,7 +5200,7 @@
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -5179,7 +5211,7 @@
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -5190,7 +5222,7 @@
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -6231,17 +6263,17 @@
     </row>
     <row r="2" ht="60.75" customHeight="1">
       <c r="A2" s="113" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="30" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="118" t="s">
-        <v>387</v>
+      <c r="A5" s="119" t="s">
+        <v>389</v>
       </c>
       <c r="B5" s="68"/>
       <c r="C5" s="68"/>
@@ -6250,7 +6282,7 @@
     </row>
     <row r="6">
       <c r="A6" s="89" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B6" s="18"/>
       <c r="E6" s="62"/>
@@ -6260,8 +6292,8 @@
       <c r="E7" s="62"/>
     </row>
     <row r="8">
-      <c r="A8" s="119" t="s">
-        <v>389</v>
+      <c r="A8" s="120" t="s">
+        <v>391</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>54</v>
@@ -6322,7 +6354,7 @@
     </row>
     <row r="14">
       <c r="A14" s="70" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -6330,7 +6362,7 @@
     </row>
     <row r="15">
       <c r="A15" s="70" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -6338,7 +6370,7 @@
     </row>
     <row r="16">
       <c r="A16" s="70" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -6355,8 +6387,8 @@
       <c r="E17" s="93"/>
     </row>
     <row r="19">
-      <c r="A19" s="120" t="s">
-        <v>393</v>
+      <c r="A19" s="121" t="s">
+        <v>395</v>
       </c>
       <c r="B19" s="68"/>
       <c r="C19" s="68"/>
@@ -6368,7 +6400,7 @@
     </row>
     <row r="20">
       <c r="A20" s="89" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B20" s="18"/>
       <c r="H20" s="62"/>
@@ -6378,8 +6410,8 @@
       <c r="H21" s="62"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="119" t="s">
-        <v>389</v>
+      <c r="A22" s="120" t="s">
+        <v>391</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>54</v>
@@ -6452,7 +6484,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="70" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -6464,12 +6496,12 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="90" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B29" s="91"/>
       <c r="C29" s="91"/>
       <c r="D29" s="91"/>
-      <c r="E29" s="121"/>
+      <c r="E29" s="122"/>
       <c r="F29" s="91"/>
       <c r="G29" s="91"/>
       <c r="H29" s="93"/>
@@ -7485,30 +7517,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B1" s="5"/>
     </row>
     <row r="2" ht="114.0" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="122" t="s">
-        <v>398</v>
-      </c>
-      <c r="B4" s="123" t="s">
-        <v>399</v>
-      </c>
-      <c r="C4" s="123" t="s">
+      <c r="A4" s="123" t="s">
+        <v>400</v>
+      </c>
+      <c r="B4" s="124" t="s">
+        <v>401</v>
+      </c>
+      <c r="C4" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="124"/>
+      <c r="D4" s="125"/>
     </row>
     <row r="5">
       <c r="A5" s="61" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="19"/>
@@ -7524,7 +7556,7 @@
     </row>
     <row r="7">
       <c r="A7" s="61" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="19"/>
@@ -7532,9 +7564,9 @@
     </row>
     <row r="8">
       <c r="A8" s="61" t="s">
-        <v>402</v>
-      </c>
-      <c r="B8" s="125"/>
+        <v>404</v>
+      </c>
+      <c r="B8" s="126"/>
       <c r="C8" s="19"/>
       <c r="D8" s="62"/>
     </row>
@@ -7546,7 +7578,7 @@
     </row>
     <row r="10">
       <c r="A10" s="82" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>207</v>
@@ -7560,31 +7592,40 @@
     </row>
     <row r="11">
       <c r="A11" s="61" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B11" s="10"/>
+      <c r="C11" s="127" t="s">
+        <v>407</v>
+      </c>
       <c r="D11" s="62"/>
     </row>
     <row r="12">
       <c r="A12" s="61" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B12" s="10"/>
+      <c r="C12" s="127" t="s">
+        <v>407</v>
+      </c>
       <c r="D12" s="62"/>
     </row>
     <row r="13">
       <c r="A13" s="61" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="B13" s="10"/>
+      <c r="C13" s="127" t="s">
+        <v>410</v>
+      </c>
       <c r="D13" s="62"/>
     </row>
     <row r="14">
-      <c r="A14" s="126" t="s">
-        <v>407</v>
+      <c r="A14" s="128" t="s">
+        <v>411</v>
       </c>
       <c r="B14" s="91"/>
-      <c r="C14" s="127"/>
+      <c r="C14" s="129"/>
       <c r="D14" s="93"/>
     </row>
     <row r="15">
@@ -7594,7 +7635,7 @@
     </row>
     <row r="16">
       <c r="A16" s="45" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>207</v>
@@ -7608,14 +7649,14 @@
     </row>
     <row r="17">
       <c r="A17" s="19" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="18"/>
     </row>
     <row r="18">
       <c r="A18" s="19" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="18"/>
@@ -9452,8 +9493,8 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="128" t="s">
-        <v>411</v>
+      <c r="A1" s="130" t="s">
+        <v>415</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="6"/>
@@ -9461,103 +9502,103 @@
       <c r="E1" s="6"/>
     </row>
     <row r="2" ht="76.5" customHeight="1">
-      <c r="A2" s="129" t="s">
-        <v>412</v>
-      </c>
-      <c r="B2" s="130"/>
-      <c r="C2" s="131"/>
+      <c r="A2" s="131" t="s">
+        <v>416</v>
+      </c>
+      <c r="B2" s="132"/>
+      <c r="C2" s="133"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="132"/>
+      <c r="A3" s="134"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="133" t="s">
-        <v>413</v>
-      </c>
-      <c r="B4" s="123" t="s">
+      <c r="A4" s="135" t="s">
+        <v>417</v>
+      </c>
+      <c r="B4" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="123" t="s">
+      <c r="C4" s="124" t="s">
         <v>207</v>
       </c>
-      <c r="D4" s="123" t="s">
+      <c r="D4" s="124" t="s">
         <v>210</v>
       </c>
-      <c r="E4" s="134" t="s">
+      <c r="E4" s="136" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="135" t="s">
-        <v>414</v>
+      <c r="A5" s="137" t="s">
+        <v>418</v>
       </c>
       <c r="B5" s="48"/>
       <c r="E5" s="62"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="135" t="s">
-        <v>415</v>
-      </c>
-      <c r="B6" s="136"/>
-      <c r="C6" s="136"/>
+      <c r="A6" s="137" t="s">
+        <v>419</v>
+      </c>
+      <c r="B6" s="138"/>
+      <c r="C6" s="138"/>
       <c r="E6" s="62"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="135" t="s">
-        <v>416</v>
+      <c r="A7" s="137" t="s">
+        <v>420</v>
       </c>
       <c r="B7" s="47"/>
       <c r="C7" s="48"/>
       <c r="E7" s="62" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="135" t="s">
-        <v>418</v>
+      <c r="A8" s="137" t="s">
+        <v>422</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="48"/>
       <c r="E8" s="62" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="135" t="s">
-        <v>419</v>
+      <c r="A9" s="137" t="s">
+        <v>423</v>
       </c>
       <c r="B9" s="47"/>
       <c r="C9" s="48"/>
       <c r="E9" s="62" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="135" t="s">
-        <v>420</v>
+      <c r="A10" s="137" t="s">
+        <v>424</v>
       </c>
       <c r="B10" s="47"/>
       <c r="E10" s="62"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="135" t="s">
-        <v>421</v>
+      <c r="A11" s="137" t="s">
+        <v>425</v>
       </c>
       <c r="B11" s="47"/>
       <c r="D11" s="47"/>
       <c r="E11" s="62"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="135" t="s">
-        <v>421</v>
+      <c r="A12" s="137" t="s">
+        <v>425</v>
       </c>
       <c r="B12" s="47"/>
       <c r="D12" s="47"/>
       <c r="E12" s="62"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="137" t="s">
-        <v>422</v>
+      <c r="A13" s="139" t="s">
+        <v>426</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>54</v>
@@ -9573,40 +9614,46 @@
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="135" t="s">
-        <v>423</v>
+      <c r="A14" s="137" t="s">
+        <v>427</v>
       </c>
       <c r="C14" s="48"/>
       <c r="E14" s="62"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="135" t="s">
-        <v>424</v>
+      <c r="A15" s="137" t="s">
+        <v>428</v>
       </c>
       <c r="B15" s="47"/>
-      <c r="C15" s="136"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="127" t="s">
+        <v>429</v>
+      </c>
       <c r="E15" s="62"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="135" t="s">
-        <v>425</v>
+      <c r="A16" s="137" t="s">
+        <v>430</v>
       </c>
       <c r="B16" s="47"/>
-      <c r="C16" s="136"/>
+      <c r="C16" s="138"/>
+      <c r="D16" s="127" t="s">
+        <v>429</v>
+      </c>
       <c r="E16" s="62"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="135" t="s">
-        <v>426</v>
-      </c>
-      <c r="C17" s="136"/>
+      <c r="A17" s="137" t="s">
+        <v>431</v>
+      </c>
+      <c r="C17" s="138"/>
       <c r="E17" s="62"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="138" t="s">
-        <v>427</v>
-      </c>
-      <c r="B18" s="121"/>
+      <c r="A18" s="140" t="s">
+        <v>432</v>
+      </c>
+      <c r="B18" s="122"/>
       <c r="C18" s="92"/>
       <c r="D18" s="92"/>
       <c r="E18" s="93"/>
@@ -9614,98 +9661,98 @@
     <row r="19" ht="14.25" customHeight="1"/>
     <row r="20" ht="14.25" customHeight="1"/>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="139" t="s">
-        <v>428</v>
-      </c>
-      <c r="B21" s="123" t="s">
+      <c r="A21" s="141" t="s">
+        <v>433</v>
+      </c>
+      <c r="B21" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="123" t="s">
+      <c r="C21" s="124" t="s">
         <v>207</v>
       </c>
-      <c r="D21" s="134" t="s">
+      <c r="D21" s="136" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="140" t="s">
-        <v>429</v>
+      <c r="A22" s="142" t="s">
+        <v>434</v>
       </c>
       <c r="B22" s="49"/>
       <c r="D22" s="62"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="140" t="s">
-        <v>430</v>
-      </c>
-      <c r="B23" s="141"/>
+      <c r="A23" s="142" t="s">
+        <v>435</v>
+      </c>
+      <c r="B23" s="143"/>
       <c r="D23" s="62"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="140" t="s">
-        <v>431</v>
+      <c r="A24" s="142" t="s">
+        <v>436</v>
       </c>
       <c r="B24" s="49"/>
       <c r="C24" s="115"/>
-      <c r="D24" s="142"/>
+      <c r="D24" s="144"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="140" t="s">
-        <v>432</v>
+      <c r="A25" s="142" t="s">
+        <v>437</v>
       </c>
       <c r="B25" s="49"/>
       <c r="C25" s="115"/>
-      <c r="D25" s="142"/>
+      <c r="D25" s="144"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="138" t="s">
-        <v>433</v>
+      <c r="A26" s="140" t="s">
+        <v>438</v>
       </c>
       <c r="B26" s="49"/>
-      <c r="C26" s="143"/>
-      <c r="D26" s="144"/>
+      <c r="C26" s="145"/>
+      <c r="D26" s="146"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="11"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="139" t="s">
-        <v>434</v>
-      </c>
-      <c r="B28" s="123" t="s">
+      <c r="A28" s="141" t="s">
+        <v>439</v>
+      </c>
+      <c r="B28" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="123" t="s">
+      <c r="C28" s="124" t="s">
         <v>207</v>
       </c>
-      <c r="D28" s="123" t="s">
+      <c r="D28" s="124" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="134" t="s">
+      <c r="E28" s="136" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="140" t="s">
-        <v>435</v>
-      </c>
-      <c r="B29" s="141"/>
+      <c r="A29" s="142" t="s">
+        <v>440</v>
+      </c>
+      <c r="B29" s="143"/>
       <c r="E29" s="62"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="140" t="s">
-        <v>436</v>
+      <c r="A30" s="142" t="s">
+        <v>441</v>
       </c>
       <c r="B30" s="47"/>
-      <c r="C30" s="145"/>
-      <c r="D30" s="146"/>
+      <c r="C30" s="147"/>
+      <c r="D30" s="148"/>
       <c r="E30" s="62"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="138" t="s">
-        <v>437</v>
-      </c>
-      <c r="B31" s="147"/>
+      <c r="A31" s="140" t="s">
+        <v>442</v>
+      </c>
+      <c r="B31" s="149"/>
       <c r="C31" s="92"/>
       <c r="D31" s="92"/>
       <c r="E31" s="93"/>
@@ -9717,115 +9764,135 @@
       <c r="A33" s="11"/>
     </row>
     <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="133" t="s">
-        <v>438</v>
-      </c>
-      <c r="B34" s="123" t="s">
+      <c r="A34" s="135" t="s">
+        <v>443</v>
+      </c>
+      <c r="B34" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="123" t="s">
+      <c r="C34" s="124" t="s">
         <v>207</v>
       </c>
-      <c r="D34" s="123" t="s">
+      <c r="D34" s="124" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="123" t="s">
+      <c r="E34" s="124" t="s">
         <v>210</v>
       </c>
-      <c r="F34" s="134" t="s">
+      <c r="F34" s="136" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="135" t="s">
-        <v>439</v>
+      <c r="A35" s="137" t="s">
+        <v>444</v>
       </c>
       <c r="B35" s="18"/>
       <c r="F35" s="62"/>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="135" t="s">
-        <v>440</v>
+      <c r="A36" s="137" t="s">
+        <v>445</v>
       </c>
       <c r="B36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="62" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="135" t="s">
-        <v>442</v>
+      <c r="A37" s="137" t="s">
+        <v>447</v>
       </c>
       <c r="C37" s="24"/>
+      <c r="D37" s="127" t="s">
+        <v>448</v>
+      </c>
       <c r="F37" s="62"/>
     </row>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="137" t="s">
-        <v>443</v>
-      </c>
+      <c r="A38" s="139" t="s">
+        <v>449</v>
+      </c>
+      <c r="D38" s="34"/>
       <c r="F38" s="62"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="135" t="s">
-        <v>404</v>
+      <c r="A39" s="137" t="s">
+        <v>406</v>
       </c>
       <c r="C39" s="24"/>
+      <c r="D39" s="127" t="s">
+        <v>407</v>
+      </c>
       <c r="F39" s="62"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="135" t="s">
-        <v>405</v>
+      <c r="A40" s="137" t="s">
+        <v>408</v>
       </c>
       <c r="C40" s="24"/>
+      <c r="D40" s="127" t="s">
+        <v>407</v>
+      </c>
       <c r="F40" s="62"/>
     </row>
     <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="137" t="s">
-        <v>444</v>
-      </c>
+      <c r="A41" s="139" t="s">
+        <v>450</v>
+      </c>
+      <c r="D41" s="34"/>
       <c r="F41" s="62"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="135" t="s">
-        <v>404</v>
+      <c r="A42" s="137" t="s">
+        <v>406</v>
       </c>
       <c r="C42" s="24"/>
+      <c r="D42" s="127" t="s">
+        <v>451</v>
+      </c>
       <c r="F42" s="62"/>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="135" t="s">
-        <v>445</v>
+      <c r="A43" s="137" t="s">
+        <v>452</v>
       </c>
       <c r="C43" s="24"/>
+      <c r="D43" s="127" t="s">
+        <v>451</v>
+      </c>
       <c r="F43" s="62"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="135" t="s">
-        <v>405</v>
+      <c r="A44" s="137" t="s">
+        <v>408</v>
       </c>
       <c r="C44" s="24"/>
+      <c r="D44" s="127" t="s">
+        <v>451</v>
+      </c>
       <c r="F44" s="62"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="135"/>
+      <c r="A45" s="137"/>
       <c r="F45" s="62"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="135" t="s">
-        <v>446</v>
-      </c>
-      <c r="B46" s="136"/>
+      <c r="A46" s="137" t="s">
+        <v>453</v>
+      </c>
+      <c r="B46" s="138"/>
       <c r="C46" s="24"/>
-      <c r="D46" s="148"/>
+      <c r="D46" s="150"/>
       <c r="F46" s="62"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="149" t="s">
-        <v>447</v>
-      </c>
-      <c r="B47" s="121"/>
-      <c r="C47" s="150"/>
+      <c r="A47" s="151" t="s">
+        <v>454</v>
+      </c>
+      <c r="B47" s="122"/>
+      <c r="C47" s="152"/>
       <c r="D47" s="92"/>
       <c r="E47" s="92"/>
       <c r="F47" s="93"/>
@@ -10886,8 +10953,8 @@
   </cols>
   <sheetData>
     <row r="1" ht="24.0" customHeight="1">
-      <c r="A1" s="151" t="s">
-        <v>448</v>
+      <c r="A1" s="153" t="s">
+        <v>455</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -10895,30 +10962,30 @@
       <c r="E1" s="6"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="152" t="s">
-        <v>449</v>
-      </c>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
+      <c r="A2" s="154" t="s">
+        <v>456</v>
+      </c>
+      <c r="B2" s="155"/>
+      <c r="C2" s="155"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="11"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="120" t="s">
-        <v>450</v>
-      </c>
-      <c r="B4" s="154"/>
-      <c r="C4" s="154"/>
-      <c r="D4" s="154"/>
-      <c r="E4" s="154"/>
-      <c r="F4" s="154"/>
+      <c r="A4" s="121" t="s">
+        <v>457</v>
+      </c>
+      <c r="B4" s="156"/>
+      <c r="C4" s="156"/>
+      <c r="D4" s="156"/>
+      <c r="E4" s="156"/>
+      <c r="F4" s="156"/>
       <c r="G4" s="68"/>
       <c r="H4" s="69"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="155" t="s">
-        <v>451</v>
+      <c r="A5" s="157" t="s">
+        <v>458</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>54</v>
@@ -10943,7 +11010,7 @@
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="156" t="s">
+      <c r="A6" s="158" t="s">
         <v>247</v>
       </c>
       <c r="H6" s="62"/>
@@ -10969,8 +11036,8 @@
       <c r="H8" s="62"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="155" t="s">
-        <v>452</v>
+      <c r="A9" s="157" t="s">
+        <v>459</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>54</v>
@@ -10991,7 +11058,7 @@
       <c r="H9" s="62"/>
     </row>
     <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="157" t="s">
+      <c r="A10" s="159" t="s">
         <v>305</v>
       </c>
       <c r="B10" s="8"/>
@@ -11089,7 +11156,7 @@
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="70" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -11099,7 +11166,7 @@
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="70" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -11109,7 +11176,7 @@
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="70" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -11118,8 +11185,8 @@
       <c r="H21" s="62"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="155" t="s">
-        <v>455</v>
+      <c r="A22" s="157" t="s">
+        <v>462</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>54</v>
@@ -11148,8 +11215,8 @@
       <c r="H23" s="62"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="157" t="s">
-        <v>456</v>
+      <c r="A24" s="159" t="s">
+        <v>463</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>54</v>
@@ -11170,7 +11237,7 @@
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="70" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -11181,7 +11248,7 @@
     </row>
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="70" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -11192,7 +11259,7 @@
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="70" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -11204,7 +11271,7 @@
     <row r="28" ht="14.25" customHeight="1">
       <c r="A28" s="70"/>
       <c r="B28" s="6" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>207</v>
@@ -11222,7 +11289,7 @@
     </row>
     <row r="29" ht="14.25" customHeight="1">
       <c r="A29" s="70" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="10"/>
@@ -11230,27 +11297,27 @@
       <c r="H29" s="62"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="155" t="s">
-        <v>458</v>
+      <c r="A30" s="157" t="s">
+        <v>465</v>
       </c>
       <c r="H30" s="62"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="157" t="s">
-        <v>459</v>
+      <c r="A31" s="159" t="s">
+        <v>466</v>
       </c>
       <c r="H31" s="62"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="89" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B32" s="18"/>
       <c r="H32" s="62"/>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="119" t="s">
-        <v>389</v>
+      <c r="A33" s="120" t="s">
+        <v>391</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>54</v>
@@ -11317,36 +11384,36 @@
     </row>
     <row r="38" ht="14.25" customHeight="1">
       <c r="A38" s="70" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="B38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="11" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="H38" s="62"/>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="70" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="B39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="11" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="H39" s="62"/>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="90" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="B40" s="91"/>
       <c r="C40" s="92"/>
       <c r="D40" s="92"/>
       <c r="E40" s="91"/>
       <c r="F40" s="92" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="G40" s="92"/>
       <c r="H40" s="93"/>
@@ -11355,78 +11422,78 @@
       <c r="A41" s="11"/>
     </row>
     <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="120" t="s">
-        <v>464</v>
-      </c>
-      <c r="B42" s="123" t="s">
+      <c r="A42" s="121" t="s">
+        <v>471</v>
+      </c>
+      <c r="B42" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="123" t="s">
+      <c r="C42" s="124" t="s">
         <v>207</v>
       </c>
-      <c r="D42" s="123" t="s">
+      <c r="D42" s="124" t="s">
         <v>56</v>
       </c>
-      <c r="E42" s="123" t="s">
+      <c r="E42" s="124" t="s">
         <v>208</v>
       </c>
-      <c r="F42" s="123" t="s">
+      <c r="F42" s="124" t="s">
         <v>209</v>
       </c>
-      <c r="G42" s="123" t="s">
+      <c r="G42" s="124" t="s">
         <v>76</v>
       </c>
-      <c r="H42" s="134" t="s">
+      <c r="H42" s="136" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="158" t="s">
-        <v>465</v>
+      <c r="A43" s="160" t="s">
+        <v>472</v>
       </c>
       <c r="H43" s="62"/>
     </row>
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="61" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="C44" s="10"/>
       <c r="H44" s="62"/>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="61" t="s">
-        <v>467</v>
-      </c>
-      <c r="B45" s="153"/>
+        <v>474</v>
+      </c>
+      <c r="B45" s="155"/>
       <c r="C45" s="10"/>
       <c r="H45" s="62"/>
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="61" t="s">
-        <v>468</v>
-      </c>
-      <c r="B46" s="153"/>
+        <v>475</v>
+      </c>
+      <c r="B46" s="155"/>
       <c r="C46" s="10"/>
       <c r="H46" s="62"/>
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="61" t="s">
-        <v>468</v>
-      </c>
-      <c r="B47" s="153"/>
+        <v>475</v>
+      </c>
+      <c r="B47" s="155"/>
       <c r="C47" s="10"/>
       <c r="H47" s="62"/>
     </row>
     <row r="48" ht="14.25" customHeight="1">
       <c r="A48" s="61"/>
-      <c r="B48" s="153"/>
-      <c r="C48" s="153"/>
-      <c r="D48" s="153"/>
+      <c r="B48" s="155"/>
+      <c r="C48" s="155"/>
+      <c r="D48" s="155"/>
       <c r="H48" s="62"/>
     </row>
     <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="155" t="s">
-        <v>451</v>
+      <c r="A49" s="157" t="s">
+        <v>458</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>54</v>
@@ -11451,7 +11518,7 @@
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="156" t="s">
+      <c r="A50" s="158" t="s">
         <v>247</v>
       </c>
       <c r="H50" s="62"/>
@@ -11475,8 +11542,8 @@
       <c r="H52" s="62"/>
     </row>
     <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="155" t="s">
-        <v>455</v>
+      <c r="A53" s="157" t="s">
+        <v>462</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>54</v>
@@ -11505,8 +11572,8 @@
       <c r="H54" s="62"/>
     </row>
     <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="157" t="s">
-        <v>456</v>
+      <c r="A55" s="159" t="s">
+        <v>463</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>54</v>
@@ -11527,7 +11594,7 @@
     </row>
     <row r="56" ht="14.25" customHeight="1">
       <c r="A56" s="70" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
@@ -11538,7 +11605,7 @@
     </row>
     <row r="57" ht="14.25" customHeight="1">
       <c r="A57" s="70" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
@@ -11549,7 +11616,7 @@
     </row>
     <row r="58" ht="14.25" customHeight="1">
       <c r="A58" s="70" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
@@ -11561,7 +11628,7 @@
     <row r="59" ht="14.25" customHeight="1">
       <c r="A59" s="70"/>
       <c r="B59" s="6" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>207</v>
@@ -11579,7 +11646,7 @@
     </row>
     <row r="60" ht="14.25" customHeight="1">
       <c r="A60" s="90" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B60" s="18"/>
       <c r="C60" s="91"/>
@@ -11611,8 +11678,8 @@
       </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
-      <c r="A63" s="159" t="s">
-        <v>469</v>
+      <c r="A63" s="161" t="s">
+        <v>476</v>
       </c>
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
@@ -11621,22 +11688,22 @@
       <c r="A64" s="11"/>
     </row>
     <row r="65" ht="14.25" customHeight="1">
-      <c r="A65" s="120" t="s">
-        <v>470</v>
-      </c>
-      <c r="B65" s="123" t="s">
+      <c r="A65" s="121" t="s">
+        <v>477</v>
+      </c>
+      <c r="B65" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="C65" s="123" t="s">
+      <c r="C65" s="124" t="s">
         <v>207</v>
       </c>
-      <c r="D65" s="123" t="s">
+      <c r="D65" s="124" t="s">
         <v>56</v>
       </c>
-      <c r="E65" s="123" t="s">
+      <c r="E65" s="124" t="s">
         <v>210</v>
       </c>
-      <c r="F65" s="123" t="s">
+      <c r="F65" s="124" t="s">
         <v>4</v>
       </c>
       <c r="G65" s="68"/>
@@ -11644,16 +11711,16 @@
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="61" t="s">
-        <v>471</v>
-      </c>
-      <c r="B66" s="153"/>
+        <v>478</v>
+      </c>
+      <c r="B66" s="155"/>
       <c r="C66" s="10"/>
       <c r="D66" s="49"/>
       <c r="H66" s="62"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
-      <c r="A67" s="155" t="s">
-        <v>451</v>
+      <c r="A67" s="157" t="s">
+        <v>458</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>54</v>
@@ -11678,7 +11745,7 @@
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
-      <c r="A68" s="156" t="s">
+      <c r="A68" s="158" t="s">
         <v>247</v>
       </c>
       <c r="H68" s="62"/>
@@ -11703,8 +11770,8 @@
       <c r="H70" s="62"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
-      <c r="A71" s="155" t="s">
-        <v>452</v>
+      <c r="A71" s="157" t="s">
+        <v>459</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>54</v>
@@ -11724,7 +11791,7 @@
       <c r="H71" s="62"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="157" t="s">
+      <c r="A72" s="159" t="s">
         <v>305</v>
       </c>
       <c r="G72" s="11"/>
@@ -11732,7 +11799,7 @@
     </row>
     <row r="73" ht="14.25" customHeight="1">
       <c r="A73" s="70" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
@@ -11743,7 +11810,7 @@
     </row>
     <row r="74" ht="14.25" customHeight="1">
       <c r="A74" s="70" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
@@ -11754,7 +11821,7 @@
     </row>
     <row r="75" ht="14.25" customHeight="1">
       <c r="A75" s="70" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="B75" s="10"/>
       <c r="C75" s="10"/>
@@ -11764,8 +11831,8 @@
       <c r="H75" s="62"/>
     </row>
     <row r="76" ht="14.25" customHeight="1">
-      <c r="A76" s="160" t="s">
-        <v>475</v>
+      <c r="A76" s="162" t="s">
+        <v>482</v>
       </c>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
@@ -11845,7 +11912,7 @@
     </row>
     <row r="83" ht="14.25" customHeight="1">
       <c r="A83" s="70" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
@@ -11855,7 +11922,7 @@
     </row>
     <row r="84" ht="14.25" customHeight="1">
       <c r="A84" s="70" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
@@ -11865,7 +11932,7 @@
     </row>
     <row r="85" ht="14.25" customHeight="1">
       <c r="A85" s="70" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
@@ -11874,8 +11941,8 @@
       <c r="H85" s="62"/>
     </row>
     <row r="86" ht="14.25" customHeight="1">
-      <c r="A86" s="155" t="s">
-        <v>455</v>
+      <c r="A86" s="157" t="s">
+        <v>462</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>54</v>
@@ -11904,8 +11971,8 @@
       <c r="H87" s="62"/>
     </row>
     <row r="88" ht="14.25" customHeight="1">
-      <c r="A88" s="157" t="s">
-        <v>456</v>
+      <c r="A88" s="159" t="s">
+        <v>463</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>54</v>
@@ -11926,7 +11993,7 @@
     </row>
     <row r="89" ht="14.25" customHeight="1">
       <c r="A89" s="70" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
@@ -11937,7 +12004,7 @@
     </row>
     <row r="90" ht="14.25" customHeight="1">
       <c r="A90" s="70" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="B90" s="10"/>
       <c r="C90" s="10"/>
@@ -11948,7 +12015,7 @@
     </row>
     <row r="91" ht="14.25" customHeight="1">
       <c r="A91" s="70" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B91" s="10"/>
       <c r="C91" s="10"/>
@@ -11960,7 +12027,7 @@
     <row r="92" ht="14.25" customHeight="1">
       <c r="A92" s="70"/>
       <c r="B92" s="6" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>207</v>
@@ -11978,7 +12045,7 @@
     </row>
     <row r="93" ht="14.25" customHeight="1">
       <c r="A93" s="70" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B93" s="18"/>
       <c r="C93" s="10"/>
@@ -11986,27 +12053,27 @@
       <c r="H93" s="62"/>
     </row>
     <row r="94" ht="14.25" customHeight="1">
-      <c r="A94" s="155" t="s">
-        <v>458</v>
+      <c r="A94" s="157" t="s">
+        <v>465</v>
       </c>
       <c r="H94" s="62"/>
     </row>
     <row r="95" ht="14.25" customHeight="1">
-      <c r="A95" s="157" t="s">
-        <v>459</v>
+      <c r="A95" s="159" t="s">
+        <v>466</v>
       </c>
       <c r="H95" s="62"/>
     </row>
     <row r="96" ht="14.25" customHeight="1">
       <c r="A96" s="89" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="B96" s="18"/>
       <c r="H96" s="62"/>
     </row>
     <row r="97" ht="14.25" customHeight="1">
-      <c r="A97" s="119" t="s">
-        <v>389</v>
+      <c r="A97" s="120" t="s">
+        <v>391</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>54</v>
@@ -12073,36 +12140,36 @@
     </row>
     <row r="102" ht="14.25" customHeight="1">
       <c r="A102" s="70" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="B102" s="10"/>
       <c r="E102" s="10"/>
       <c r="F102" s="11" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="H102" s="62"/>
     </row>
     <row r="103" ht="14.25" customHeight="1">
       <c r="A103" s="70" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="B103" s="10"/>
       <c r="E103" s="10"/>
       <c r="F103" s="11" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="H103" s="62"/>
     </row>
     <row r="104" ht="14.25" customHeight="1">
       <c r="A104" s="90" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="B104" s="91"/>
       <c r="C104" s="92"/>
       <c r="D104" s="92"/>
       <c r="E104" s="91"/>
       <c r="F104" s="92" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="G104" s="92"/>
       <c r="H104" s="93"/>
@@ -13463,22 +13530,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="8" t="s">
-        <v>476</v>
+        <v>483</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>477</v>
-      </c>
-      <c r="C1" s="161" t="s">
-        <v>478</v>
+        <v>484</v>
+      </c>
+      <c r="C1" s="163" t="s">
+        <v>485</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>51</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>208</v>
@@ -13486,196 +13553,196 @@
     </row>
     <row r="3">
       <c r="A3" s="16" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>482</v>
+        <v>489</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="16" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="16" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
     </row>
     <row r="7">
       <c r="C7" s="19" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
     </row>
     <row r="8">
       <c r="C8" s="19" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
     </row>
     <row r="9">
       <c r="F9" s="16" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="8" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
     </row>
     <row r="11">
       <c r="F11" s="16" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="16" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>526</v>
+        <v>533</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="19" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="16" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>69</v>
@@ -13683,242 +13750,242 @@
     </row>
     <row r="17">
       <c r="A17" s="16" t="s">
-        <v>531</v>
+        <v>538</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="16" t="s">
-        <v>532</v>
+        <v>539</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>534</v>
+        <v>541</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
-        <v>535</v>
+        <v>542</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>536</v>
+        <v>543</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="16" t="s">
-        <v>537</v>
+        <v>544</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>538</v>
+        <v>545</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="16" t="s">
-        <v>542</v>
+        <v>549</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="16" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>544</v>
+        <v>551</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>546</v>
+        <v>553</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>547</v>
+        <v>554</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="16" t="s">
-        <v>548</v>
+        <v>555</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>549</v>
+        <v>556</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>550</v>
+        <v>557</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>551</v>
+        <v>558</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>552</v>
+        <v>559</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>553</v>
+        <v>560</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="16" t="s">
-        <v>554</v>
+        <v>561</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>555</v>
+        <v>562</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>556</v>
+        <v>563</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>557</v>
+        <v>564</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>558</v>
+        <v>565</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="16" t="s">
-        <v>559</v>
+        <v>566</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>560</v>
+        <v>567</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>562</v>
+        <v>569</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>563</v>
+        <v>570</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="16" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>567</v>
+        <v>574</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="16" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>570</v>
+        <v>577</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="16" t="s">
-        <v>572</v>
+        <v>579</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>573</v>
+        <v>580</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="16" t="s">
-        <v>574</v>
+        <v>581</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="16" t="s">
-        <v>575</v>
+        <v>582</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>576</v>
+        <v>583</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="16" t="s">
-        <v>577</v>
+        <v>584</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>578</v>
+        <v>585</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>580</v>
+        <v>587</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="E34" s="19" t="s">
-        <v>581</v>
+        <v>588</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="16" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>583</v>
+        <v>590</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>584</v>
+        <v>591</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="16" t="s">
-        <v>585</v>
+        <v>592</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>586</v>
+        <v>593</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>587</v>
+        <v>594</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="16" t="s">
-        <v>588</v>
+        <v>595</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>589</v>
+        <v>596</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>590</v>
+        <v>597</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="16" t="s">
-        <v>591</v>
+        <v>598</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>592</v>
+        <v>599</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="B39" s="16" t="s">
-        <v>593</v>
+        <v>600</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
@@ -13926,304 +13993,304 @@
         <v>331</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>594</v>
+        <v>601</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="E41" s="19" t="s">
-        <v>595</v>
+        <v>602</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="16" t="s">
-        <v>596</v>
+        <v>603</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>597</v>
+        <v>604</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="16" t="s">
-        <v>598</v>
+        <v>605</v>
       </c>
       <c r="E43" s="19" t="s">
-        <v>599</v>
+        <v>606</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1"/>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="8" t="s">
-        <v>600</v>
+        <v>607</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>601</v>
+        <v>608</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>602</v>
+        <v>609</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1"/>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="19" t="s">
-        <v>603</v>
+        <v>610</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>604</v>
+        <v>611</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>605</v>
+        <v>612</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>606</v>
+        <v>613</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="19" t="s">
-        <v>607</v>
+        <v>614</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>608</v>
+        <v>615</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>609</v>
+        <v>616</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>610</v>
+        <v>617</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="19" t="s">
-        <v>611</v>
+        <v>618</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>612</v>
+        <v>619</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>613</v>
+        <v>620</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="19" t="s">
-        <v>614</v>
+        <v>621</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="19" t="s">
-        <v>615</v>
+        <v>622</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="19" t="s">
-        <v>616</v>
+        <v>623</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="19" t="s">
-        <v>617</v>
+        <v>624</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1"/>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="8" t="s">
-        <v>618</v>
+        <v>625</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1"/>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="19" t="s">
-        <v>619</v>
+        <v>626</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="16" t="s">
-        <v>620</v>
+        <v>627</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="19" t="s">
-        <v>621</v>
+        <v>628</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1"/>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="8" t="s">
-        <v>622</v>
+        <v>629</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>623</v>
+        <v>630</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>624</v>
+        <v>631</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>625</v>
+        <v>632</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>626</v>
+        <v>633</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>627</v>
+        <v>634</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>628</v>
+        <v>635</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="19" t="s">
-        <v>629</v>
+        <v>636</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>630</v>
+        <v>637</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>631</v>
+        <v>638</v>
       </c>
       <c r="D63" s="19" t="s">
-        <v>632</v>
+        <v>639</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>633</v>
+        <v>640</v>
       </c>
       <c r="F63" s="16" t="s">
-        <v>634</v>
+        <v>641</v>
       </c>
       <c r="G63" s="19" t="s">
-        <v>635</v>
+        <v>642</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="19" t="s">
-        <v>636</v>
+        <v>643</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>637</v>
+        <v>644</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>638</v>
+        <v>645</v>
       </c>
       <c r="D64" s="19" t="s">
-        <v>639</v>
+        <v>646</v>
       </c>
       <c r="E64" s="16" t="s">
-        <v>640</v>
+        <v>647</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>641</v>
+        <v>648</v>
       </c>
       <c r="G64" s="19" t="s">
-        <v>642</v>
+        <v>649</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="19" t="s">
-        <v>643</v>
+        <v>650</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>644</v>
+        <v>651</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>645</v>
+        <v>652</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>646</v>
+        <v>653</v>
       </c>
       <c r="E65" s="16" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>648</v>
+        <v>655</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="19" t="s">
-        <v>649</v>
+        <v>656</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>650</v>
+        <v>657</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>651</v>
+        <v>658</v>
       </c>
       <c r="E66" s="16" t="s">
-        <v>652</v>
+        <v>659</v>
       </c>
       <c r="F66" s="16" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="B67" s="19" t="s">
-        <v>654</v>
+        <v>661</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>655</v>
+        <v>662</v>
       </c>
       <c r="E67" s="16" t="s">
-        <v>656</v>
+        <v>663</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="B68" s="19" t="s">
-        <v>657</v>
+        <v>664</v>
       </c>
       <c r="E68" s="16" t="s">
-        <v>658</v>
+        <v>665</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="B69" s="19" t="s">
-        <v>659</v>
+        <v>666</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>660</v>
+        <v>667</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="B70" s="19" t="s">
-        <v>661</v>
+        <v>668</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="8" t="s">
-        <v>662</v>
+        <v>669</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1"/>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="19" t="s">
-        <v>664</v>
+        <v>671</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>665</v>
+        <v>672</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="19" t="s">
-        <v>666</v>
+        <v>673</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>667</v>
+        <v>674</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="19" t="s">
-        <v>668</v>
+        <v>675</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>669</v>
+        <v>676</v>
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="19" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1"/>
@@ -14526,296 +14593,296 @@
     <row r="375" ht="15.75" customHeight="1"/>
     <row r="376" ht="15.75" customHeight="1">
       <c r="A376" s="16" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c r="B376" s="16" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="C376" s="19" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
     </row>
     <row r="377" ht="15.75" customHeight="1">
       <c r="A377" s="16" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="B377" s="16" t="s">
-        <v>671</v>
+        <v>678</v>
       </c>
       <c r="C377" s="19" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
     </row>
     <row r="378" ht="15.75" customHeight="1">
       <c r="A378" s="16" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="C378" s="19" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
     </row>
     <row r="379" ht="15.75" customHeight="1">
       <c r="C379" s="19" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
     </row>
     <row r="380" ht="15.75" customHeight="1">
       <c r="C380" s="19" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
     </row>
     <row r="381" ht="15.75" customHeight="1"/>
     <row r="382" ht="15.75" customHeight="1">
       <c r="A382" s="8" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="B382" s="8" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="C382" s="8" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="D382" s="8" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
     </row>
     <row r="383" ht="15.75" customHeight="1"/>
     <row r="384" ht="15.75" customHeight="1">
       <c r="A384" s="16" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="B384" s="19" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="C384" s="19" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="D384" s="16" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
     </row>
     <row r="385" ht="15.75" customHeight="1">
       <c r="A385" s="16" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="B385" s="19" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="C385" s="19" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="D385" s="16" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
     </row>
     <row r="386" ht="15.75" customHeight="1">
       <c r="A386" s="16" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="B386" s="19" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="C386" s="19" t="s">
-        <v>526</v>
+        <v>533</v>
       </c>
       <c r="D386" s="16" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
     </row>
     <row r="387" ht="15.75" customHeight="1">
       <c r="A387" s="16" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="B387" s="19"/>
       <c r="C387" s="19" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
     </row>
     <row r="388" ht="15.75" customHeight="1">
       <c r="A388" s="16" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
       <c r="C388" s="19" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
     </row>
     <row r="389" ht="15.75" customHeight="1">
       <c r="A389" s="16" t="s">
-        <v>531</v>
+        <v>538</v>
       </c>
       <c r="B389" s="16" t="s">
-        <v>672</v>
+        <v>679</v>
       </c>
       <c r="C389" s="19" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
     </row>
     <row r="390" ht="15.75" customHeight="1">
       <c r="A390" s="16" t="s">
-        <v>532</v>
+        <v>539</v>
       </c>
       <c r="C390" s="19" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
     </row>
     <row r="391" ht="15.75" customHeight="1">
       <c r="A391" s="16" t="s">
-        <v>535</v>
+        <v>542</v>
       </c>
     </row>
     <row r="392" ht="15.75" customHeight="1">
       <c r="A392" s="16" t="s">
-        <v>537</v>
+        <v>544</v>
       </c>
       <c r="B392" s="8" t="s">
-        <v>538</v>
+        <v>545</v>
       </c>
       <c r="C392" s="8" t="s">
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="D392" s="8" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
     </row>
     <row r="393" ht="15.75" customHeight="1">
       <c r="A393" s="16" t="s">
-        <v>542</v>
+        <v>549</v>
       </c>
     </row>
     <row r="394" ht="15.75" customHeight="1">
       <c r="A394" s="16" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
       <c r="B394" s="16" t="s">
-        <v>544</v>
+        <v>551</v>
       </c>
       <c r="C394" s="19" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="D394" s="16" t="s">
-        <v>546</v>
+        <v>553</v>
       </c>
     </row>
     <row r="395" ht="15.75" customHeight="1">
       <c r="A395" s="16" t="s">
-        <v>548</v>
+        <v>555</v>
       </c>
       <c r="B395" s="16" t="s">
-        <v>549</v>
+        <v>556</v>
       </c>
       <c r="C395" s="19" t="s">
-        <v>550</v>
+        <v>557</v>
       </c>
       <c r="D395" s="16" t="s">
-        <v>551</v>
+        <v>558</v>
       </c>
     </row>
     <row r="396" ht="15.75" customHeight="1">
       <c r="A396" s="16" t="s">
-        <v>554</v>
+        <v>561</v>
       </c>
       <c r="C396" s="19" t="s">
-        <v>555</v>
+        <v>562</v>
       </c>
       <c r="D396" s="16" t="s">
-        <v>556</v>
+        <v>563</v>
       </c>
     </row>
     <row r="397" ht="15.75" customHeight="1">
       <c r="A397" s="16" t="s">
-        <v>559</v>
+        <v>566</v>
       </c>
       <c r="C397" s="19" t="s">
-        <v>560</v>
+        <v>567</v>
       </c>
       <c r="D397" s="16" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
     </row>
     <row r="398" ht="15.75" customHeight="1">
       <c r="A398" s="16" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="D398" s="16" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
     </row>
     <row r="399" ht="15.75" customHeight="1">
       <c r="A399" s="16" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="D399" s="16" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
     </row>
     <row r="400" ht="15.75" customHeight="1">
       <c r="A400" s="16" t="s">
-        <v>572</v>
+        <v>579</v>
       </c>
     </row>
     <row r="401" ht="15.75" customHeight="1">
       <c r="A401" s="16" t="s">
-        <v>574</v>
+        <v>581</v>
       </c>
       <c r="B401" s="16" t="s">
-        <v>673</v>
+        <v>680</v>
       </c>
     </row>
     <row r="402" ht="15.75" customHeight="1">
       <c r="A402" s="16" t="s">
-        <v>575</v>
+        <v>582</v>
       </c>
     </row>
     <row r="403" ht="15.75" customHeight="1">
       <c r="A403" s="16" t="s">
-        <v>577</v>
+        <v>584</v>
       </c>
     </row>
     <row r="404" ht="15.75" customHeight="1"/>
     <row r="405" ht="15.75" customHeight="1">
       <c r="A405" s="8" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="B405" s="8" t="s">
-        <v>580</v>
+        <v>587</v>
       </c>
     </row>
     <row r="406" ht="15.75" customHeight="1"/>
     <row r="407" ht="15.75" customHeight="1">
       <c r="A407" s="16" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
       <c r="B407" s="16" t="s">
-        <v>583</v>
+        <v>590</v>
       </c>
     </row>
     <row r="408" ht="15.75" customHeight="1">
       <c r="A408" s="16" t="s">
-        <v>585</v>
+        <v>592</v>
       </c>
       <c r="B408" s="16" t="s">
-        <v>586</v>
+        <v>593</v>
       </c>
     </row>
     <row r="409" ht="15.75" customHeight="1">
       <c r="A409" s="16" t="s">
-        <v>588</v>
+        <v>595</v>
       </c>
       <c r="B409" s="16" t="s">
-        <v>589</v>
+        <v>596</v>
       </c>
     </row>
     <row r="410" ht="15.75" customHeight="1">
       <c r="A410" s="16" t="s">
-        <v>591</v>
+        <v>598</v>
       </c>
       <c r="B410" s="16" t="s">
-        <v>592</v>
+        <v>599</v>
       </c>
     </row>
     <row r="411" ht="15.75" customHeight="1">
       <c r="B411" s="16" t="s">
-        <v>593</v>
+        <v>600</v>
       </c>
     </row>
     <row r="412" ht="15.75" customHeight="1">
@@ -14825,251 +14892,251 @@
     </row>
     <row r="413" ht="15.75" customHeight="1">
       <c r="B413" s="16" t="s">
-        <v>674</v>
+        <v>681</v>
       </c>
     </row>
     <row r="414" ht="15.75" customHeight="1">
       <c r="A414" s="16" t="s">
-        <v>596</v>
+        <v>603</v>
       </c>
     </row>
     <row r="415" ht="15.75" customHeight="1">
       <c r="A415" s="16" t="s">
-        <v>598</v>
+        <v>605</v>
       </c>
     </row>
     <row r="416" ht="15.75" customHeight="1"/>
     <row r="417" ht="15.75" customHeight="1">
       <c r="A417" s="8" t="s">
-        <v>600</v>
+        <v>607</v>
       </c>
       <c r="B417" s="8" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C417" s="8" t="s">
-        <v>601</v>
+        <v>608</v>
       </c>
       <c r="D417" s="8" t="s">
-        <v>602</v>
+        <v>609</v>
       </c>
     </row>
     <row r="418" ht="15.75" customHeight="1"/>
     <row r="419" ht="15.75" customHeight="1">
       <c r="A419" s="19" t="s">
-        <v>603</v>
+        <v>610</v>
       </c>
       <c r="B419" s="19" t="s">
-        <v>604</v>
+        <v>611</v>
       </c>
       <c r="C419" s="16" t="s">
-        <v>605</v>
+        <v>612</v>
       </c>
       <c r="D419" s="16" t="s">
-        <v>606</v>
+        <v>613</v>
       </c>
     </row>
     <row r="420" ht="15.75" customHeight="1">
       <c r="A420" s="19" t="s">
-        <v>607</v>
+        <v>614</v>
       </c>
       <c r="B420" s="19" t="s">
-        <v>608</v>
+        <v>615</v>
       </c>
       <c r="C420" s="16" t="s">
-        <v>609</v>
+        <v>616</v>
       </c>
       <c r="D420" s="16" t="s">
-        <v>610</v>
+        <v>617</v>
       </c>
     </row>
     <row r="421" ht="15.75" customHeight="1">
       <c r="A421" s="19" t="s">
-        <v>611</v>
+        <v>618</v>
       </c>
       <c r="B421" s="19" t="s">
-        <v>612</v>
+        <v>619</v>
       </c>
       <c r="C421" s="16" t="s">
-        <v>613</v>
+        <v>620</v>
       </c>
     </row>
     <row r="422" ht="15.75" customHeight="1">
       <c r="A422" s="19" t="s">
-        <v>614</v>
+        <v>621</v>
       </c>
     </row>
     <row r="423" ht="15.75" customHeight="1">
       <c r="A423" s="19" t="s">
-        <v>615</v>
+        <v>622</v>
       </c>
     </row>
     <row r="424" ht="15.75" customHeight="1">
       <c r="A424" s="19" t="s">
-        <v>616</v>
+        <v>623</v>
       </c>
     </row>
     <row r="425" ht="15.75" customHeight="1">
       <c r="A425" s="19" t="s">
-        <v>617</v>
+        <v>624</v>
       </c>
       <c r="B425" s="16" t="s">
-        <v>675</v>
+        <v>682</v>
       </c>
     </row>
     <row r="426" ht="15.75" customHeight="1"/>
     <row r="427" ht="15.75" customHeight="1">
       <c r="A427" s="8" t="s">
-        <v>618</v>
+        <v>625</v>
       </c>
     </row>
     <row r="428" ht="15.75" customHeight="1"/>
     <row r="429" ht="15.75" customHeight="1">
       <c r="A429" s="19" t="s">
-        <v>619</v>
+        <v>626</v>
       </c>
     </row>
     <row r="430" ht="15.75" customHeight="1">
       <c r="A430" s="16" t="s">
-        <v>620</v>
+        <v>627</v>
       </c>
     </row>
     <row r="431" ht="15.75" customHeight="1">
       <c r="A431" s="19" t="s">
-        <v>621</v>
+        <v>628</v>
       </c>
     </row>
     <row r="432" ht="15.75" customHeight="1"/>
     <row r="433" ht="15.75" customHeight="1">
       <c r="A433" s="8" t="s">
-        <v>622</v>
+        <v>629</v>
       </c>
       <c r="B433" s="8" t="s">
-        <v>623</v>
+        <v>630</v>
       </c>
       <c r="C433" s="8" t="s">
-        <v>624</v>
+        <v>631</v>
       </c>
       <c r="D433" s="8" t="s">
-        <v>625</v>
+        <v>632</v>
       </c>
     </row>
     <row r="434" ht="15.75" customHeight="1"/>
     <row r="435" ht="15.75" customHeight="1">
       <c r="A435" s="19" t="s">
-        <v>629</v>
+        <v>636</v>
       </c>
       <c r="B435" s="19" t="s">
-        <v>630</v>
+        <v>637</v>
       </c>
       <c r="C435" s="19" t="s">
-        <v>631</v>
+        <v>638</v>
       </c>
       <c r="D435" s="19" t="s">
-        <v>632</v>
+        <v>639</v>
       </c>
     </row>
     <row r="436" ht="15.75" customHeight="1">
       <c r="A436" s="19" t="s">
-        <v>636</v>
+        <v>643</v>
       </c>
       <c r="B436" s="19" t="s">
-        <v>637</v>
+        <v>644</v>
       </c>
       <c r="C436" s="19" t="s">
-        <v>638</v>
+        <v>645</v>
       </c>
       <c r="D436" s="19" t="s">
-        <v>639</v>
+        <v>646</v>
       </c>
     </row>
     <row r="437" ht="15.75" customHeight="1">
       <c r="A437" s="19" t="s">
-        <v>643</v>
+        <v>650</v>
       </c>
       <c r="B437" s="19" t="s">
-        <v>676</v>
+        <v>683</v>
       </c>
       <c r="C437" s="19" t="s">
-        <v>645</v>
+        <v>652</v>
       </c>
       <c r="D437" s="16" t="s">
-        <v>646</v>
+        <v>653</v>
       </c>
     </row>
     <row r="438" ht="15.75" customHeight="1">
       <c r="A438" s="19" t="s">
-        <v>649</v>
+        <v>656</v>
       </c>
       <c r="B438" s="19" t="s">
-        <v>650</v>
+        <v>657</v>
       </c>
       <c r="D438" s="16" t="s">
-        <v>651</v>
+        <v>658</v>
       </c>
     </row>
     <row r="439" ht="15.75" customHeight="1">
       <c r="B439" s="19" t="s">
-        <v>654</v>
+        <v>661</v>
       </c>
       <c r="D439" s="16" t="s">
-        <v>655</v>
+        <v>662</v>
       </c>
     </row>
     <row r="440" ht="15.75" customHeight="1">
       <c r="B440" s="19" t="s">
-        <v>657</v>
+        <v>664</v>
       </c>
     </row>
     <row r="441" ht="15.75" customHeight="1">
       <c r="B441" s="19" t="s">
-        <v>659</v>
+        <v>666</v>
       </c>
     </row>
     <row r="442" ht="15.75" customHeight="1">
       <c r="B442" s="19" t="s">
-        <v>661</v>
+        <v>668</v>
       </c>
     </row>
     <row r="443" ht="15.75" customHeight="1"/>
     <row r="444" ht="15.75" customHeight="1">
       <c r="A444" s="8" t="s">
-        <v>662</v>
+        <v>669</v>
       </c>
       <c r="B444" s="8" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
     </row>
     <row r="445" ht="15.75" customHeight="1"/>
     <row r="446" ht="15.75" customHeight="1">
       <c r="A446" s="19" t="s">
-        <v>664</v>
+        <v>671</v>
       </c>
       <c r="B446" s="19" t="s">
-        <v>665</v>
+        <v>672</v>
       </c>
     </row>
     <row r="447" ht="15.75" customHeight="1">
       <c r="A447" s="19" t="s">
-        <v>666</v>
+        <v>673</v>
       </c>
       <c r="B447" s="19" t="s">
-        <v>667</v>
+        <v>674</v>
       </c>
     </row>
     <row r="448" ht="15.75" customHeight="1">
       <c r="A448" s="19" t="s">
-        <v>668</v>
+        <v>675</v>
       </c>
       <c r="B448" s="19" t="s">
-        <v>669</v>
+        <v>676</v>
       </c>
     </row>
     <row r="449" ht="15.75" customHeight="1">
       <c r="A449" s="19" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="B449" s="16" t="s">
-        <v>677</v>
+        <v>684</v>
       </c>
     </row>
     <row r="450" ht="15.75" customHeight="1"/>
@@ -15085,7 +15152,7 @@
     <row r="460" ht="15.75" customHeight="1"/>
     <row r="461" ht="15.75" customHeight="1">
       <c r="B461" s="16" t="s">
-        <v>678</v>
+        <v>685</v>
       </c>
     </row>
     <row r="462" ht="15.75" customHeight="1"/>
@@ -15101,7 +15168,7 @@
     <row r="472" ht="15.75" customHeight="1"/>
     <row r="473" ht="15.75" customHeight="1">
       <c r="B473" s="16" t="s">
-        <v>679</v>
+        <v>686</v>
       </c>
     </row>
     <row r="474" ht="15.75" customHeight="1"/>
@@ -15117,7 +15184,7 @@
     <row r="484" ht="15.75" customHeight="1"/>
     <row r="485" ht="15.75" customHeight="1">
       <c r="B485" s="16" t="s">
-        <v>680</v>
+        <v>687</v>
       </c>
     </row>
     <row r="486" ht="15.75" customHeight="1"/>
@@ -15133,7 +15200,7 @@
     <row r="496" ht="15.75" customHeight="1"/>
     <row r="497" ht="15.75" customHeight="1">
       <c r="B497" s="16" t="s">
-        <v>681</v>
+        <v>688</v>
       </c>
     </row>
     <row r="498" ht="15.75" customHeight="1"/>
@@ -15149,7 +15216,7 @@
     <row r="508" ht="15.75" customHeight="1"/>
     <row r="509" ht="15.75" customHeight="1">
       <c r="B509" s="16" t="s">
-        <v>682</v>
+        <v>689</v>
       </c>
     </row>
     <row r="510" ht="15.75" customHeight="1"/>
@@ -15165,7 +15232,7 @@
     <row r="520" ht="15.75" customHeight="1"/>
     <row r="521" ht="15.75" customHeight="1">
       <c r="B521" s="16" t="s">
-        <v>683</v>
+        <v>690</v>
       </c>
     </row>
     <row r="522" ht="15.75" customHeight="1"/>
@@ -15181,7 +15248,7 @@
     <row r="532" ht="15.75" customHeight="1"/>
     <row r="533" ht="15.75" customHeight="1">
       <c r="B533" s="16" t="s">
-        <v>684</v>
+        <v>691</v>
       </c>
     </row>
     <row r="534" ht="15.75" customHeight="1"/>
@@ -15197,7 +15264,7 @@
     <row r="544" ht="15.75" customHeight="1"/>
     <row r="545" ht="15.75" customHeight="1">
       <c r="B545" s="16" t="s">
-        <v>685</v>
+        <v>692</v>
       </c>
     </row>
     <row r="546" ht="15.75" customHeight="1"/>
@@ -15213,7 +15280,7 @@
     <row r="556" ht="15.75" customHeight="1"/>
     <row r="557" ht="15.75" customHeight="1">
       <c r="B557" s="16" t="s">
-        <v>686</v>
+        <v>693</v>
       </c>
     </row>
     <row r="558" ht="15.75" customHeight="1"/>
@@ -15229,7 +15296,7 @@
     <row r="568" ht="15.75" customHeight="1"/>
     <row r="569" ht="15.75" customHeight="1">
       <c r="B569" s="16" t="s">
-        <v>687</v>
+        <v>694</v>
       </c>
     </row>
     <row r="570" ht="15.75" customHeight="1"/>
@@ -15245,7 +15312,7 @@
     <row r="580" ht="15.75" customHeight="1"/>
     <row r="581" ht="15.75" customHeight="1">
       <c r="B581" s="16" t="s">
-        <v>688</v>
+        <v>695</v>
       </c>
     </row>
     <row r="582" ht="15.75" customHeight="1"/>
@@ -15261,7 +15328,7 @@
     <row r="592" ht="15.75" customHeight="1"/>
     <row r="593" ht="15.75" customHeight="1">
       <c r="B593" s="16" t="s">
-        <v>689</v>
+        <v>696</v>
       </c>
     </row>
     <row r="594" ht="15.75" customHeight="1"/>
@@ -15277,7 +15344,7 @@
     <row r="604" ht="15.75" customHeight="1"/>
     <row r="605" ht="15.75" customHeight="1">
       <c r="B605" s="16" t="s">
-        <v>690</v>
+        <v>697</v>
       </c>
     </row>
     <row r="606" ht="15.75" customHeight="1"/>
@@ -15293,7 +15360,7 @@
     <row r="616" ht="15.75" customHeight="1"/>
     <row r="617" ht="15.75" customHeight="1">
       <c r="B617" s="16" t="s">
-        <v>691</v>
+        <v>698</v>
       </c>
     </row>
     <row r="618" ht="15.75" customHeight="1"/>
@@ -15309,7 +15376,7 @@
     <row r="628" ht="15.75" customHeight="1"/>
     <row r="629" ht="15.75" customHeight="1">
       <c r="B629" s="16" t="s">
-        <v>692</v>
+        <v>699</v>
       </c>
     </row>
     <row r="630" ht="15.75" customHeight="1"/>
@@ -15325,7 +15392,7 @@
     <row r="640" ht="15.75" customHeight="1"/>
     <row r="641" ht="15.75" customHeight="1">
       <c r="B641" s="16" t="s">
-        <v>693</v>
+        <v>700</v>
       </c>
     </row>
     <row r="642" ht="15.75" customHeight="1"/>
@@ -15341,7 +15408,7 @@
     <row r="652" ht="15.75" customHeight="1"/>
     <row r="653" ht="15.75" customHeight="1">
       <c r="B653" s="16" t="s">
-        <v>694</v>
+        <v>701</v>
       </c>
     </row>
     <row r="654" ht="15.75" customHeight="1"/>
@@ -15357,7 +15424,7 @@
     <row r="664" ht="15.75" customHeight="1"/>
     <row r="665" ht="15.75" customHeight="1">
       <c r="B665" s="16" t="s">
-        <v>695</v>
+        <v>702</v>
       </c>
     </row>
     <row r="666" ht="15.75" customHeight="1"/>
@@ -15373,7 +15440,7 @@
     <row r="676" ht="15.75" customHeight="1"/>
     <row r="677" ht="15.75" customHeight="1">
       <c r="B677" s="16" t="s">
-        <v>696</v>
+        <v>703</v>
       </c>
     </row>
     <row r="678" ht="15.75" customHeight="1"/>
@@ -15389,7 +15456,7 @@
     <row r="688" ht="15.75" customHeight="1"/>
     <row r="689" ht="15.75" customHeight="1">
       <c r="B689" s="16" t="s">
-        <v>697</v>
+        <v>704</v>
       </c>
     </row>
     <row r="690" ht="15.75" customHeight="1"/>
@@ -15405,7 +15472,7 @@
     <row r="700" ht="15.75" customHeight="1"/>
     <row r="701" ht="15.75" customHeight="1">
       <c r="B701" s="16" t="s">
-        <v>698</v>
+        <v>705</v>
       </c>
     </row>
     <row r="702" ht="15.75" customHeight="1"/>
@@ -15421,7 +15488,7 @@
     <row r="712" ht="15.75" customHeight="1"/>
     <row r="713" ht="15.75" customHeight="1">
       <c r="B713" s="16" t="s">
-        <v>699</v>
+        <v>706</v>
       </c>
     </row>
     <row r="714" ht="15.75" customHeight="1"/>
@@ -15437,7 +15504,7 @@
     <row r="724" ht="15.75" customHeight="1"/>
     <row r="725" ht="15.75" customHeight="1">
       <c r="B725" s="16" t="s">
-        <v>700</v>
+        <v>707</v>
       </c>
     </row>
     <row r="726" ht="15.75" customHeight="1"/>
@@ -15453,7 +15520,7 @@
     <row r="736" ht="15.75" customHeight="1"/>
     <row r="737" ht="15.75" customHeight="1">
       <c r="B737" s="16" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
     </row>
     <row r="738" ht="15.75" customHeight="1"/>
@@ -15750,7 +15817,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>701</v>
+        <v>708</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="6"/>
@@ -15782,7 +15849,7 @@
     </row>
     <row r="2" ht="60.0" customHeight="1">
       <c r="A2" s="113" t="s">
-        <v>702</v>
+        <v>709</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
@@ -15820,8 +15887,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="162" t="s">
-        <v>703</v>
+      <c r="A5" s="164" t="s">
+        <v>710</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>54</v>
@@ -15874,8 +15941,8 @@
       <c r="E9" s="16"/>
     </row>
     <row r="10">
-      <c r="A10" s="162" t="s">
-        <v>704</v>
+      <c r="A10" s="164" t="s">
+        <v>711</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>54</v>
@@ -15935,8 +16002,8 @@
       <c r="E15" s="16"/>
     </row>
     <row r="16">
-      <c r="A16" s="162" t="s">
-        <v>705</v>
+      <c r="A16" s="164" t="s">
+        <v>712</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>54</v>
@@ -15994,8 +16061,8 @@
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="162" t="s">
-        <v>706</v>
+      <c r="A22" s="164" t="s">
+        <v>713</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>54</v>
@@ -16048,8 +16115,8 @@
       <c r="A26" s="19"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="162" t="s">
-        <v>707</v>
+      <c r="A27" s="164" t="s">
+        <v>714</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>54</v>
@@ -16103,8 +16170,8 @@
       <c r="E31" s="16"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="162" t="s">
-        <v>708</v>
+      <c r="A32" s="164" t="s">
+        <v>715</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>54</v>
@@ -16162,8 +16229,8 @@
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="162" t="s">
-        <v>709</v>
+      <c r="A38" s="164" t="s">
+        <v>716</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>54</v>
@@ -16267,8 +16334,8 @@
       <c r="Y42" s="19"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="162" t="s">
-        <v>710</v>
+      <c r="A43" s="164" t="s">
+        <v>717</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>54</v>
@@ -33278,19 +33345,29 @@
       <c r="C18" s="10"/>
       <c r="D18" s="18"/>
       <c r="E18" s="10"/>
+      <c r="F18" s="118" t="s">
+        <v>345</v>
+      </c>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
     </row>
     <row r="19">
       <c r="A19" s="115" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
+      <c r="F19" s="118" t="s">
+        <v>347</v>
+      </c>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20">
       <c r="A20" s="16" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -33300,7 +33377,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="16" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -33310,7 +33387,7 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="16" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -33328,7 +33405,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="B24" s="6" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>207</v>
@@ -33345,7 +33422,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="16" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="10"/>
@@ -33365,7 +33442,7 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="16" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -33383,14 +33460,14 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="16" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="16" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -34417,12 +34494,12 @@
     </row>
     <row r="2" ht="60.75" customHeight="1">
       <c r="A2" s="113" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="30" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5">
@@ -34432,7 +34509,7 @@
     </row>
     <row r="6">
       <c r="A6" s="45" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B6" s="10"/>
     </row>
@@ -34464,13 +34541,13 @@
     </row>
     <row r="9">
       <c r="A9" s="45" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B9" s="10"/>
     </row>
     <row r="11">
       <c r="A11" s="45" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>54</v>
@@ -34496,14 +34573,14 @@
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -34514,7 +34591,7 @@
     </row>
     <row r="14">
       <c r="A14" s="16" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -34525,7 +34602,7 @@
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -34536,7 +34613,7 @@
     </row>
     <row r="16">
       <c r="A16" s="16" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -34547,7 +34624,7 @@
     </row>
     <row r="18">
       <c r="A18" s="45" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -34558,7 +34635,7 @@
     </row>
     <row r="20">
       <c r="A20" s="45" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -34570,7 +34647,7 @@
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="45" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -34582,7 +34659,7 @@
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="45" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -34594,7 +34671,7 @@
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="45" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -34608,7 +34685,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="45" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -34622,7 +34699,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="45" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -34636,7 +34713,7 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="45" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -34650,7 +34727,7 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="45" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -34664,7 +34741,7 @@
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="45" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -34678,7 +34755,7 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="45" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -34692,7 +34769,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="45" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>

</xml_diff>